<commit_message>
new working files added
</commit_message>
<xml_diff>
--- a/CSV spreadsheet/nei.j4b.xlsx
+++ b/CSV spreadsheet/nei.j4b.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4780" uniqueCount="2404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4798" uniqueCount="2405">
   <si>
     <t xml:space="preserve">Filename </t>
   </si>
@@ -7231,6 +7231,9 @@
   </si>
   <si>
     <t>AM (no xml)</t>
+  </si>
+  <si>
+    <t>pages 81 and 82 are missing</t>
   </si>
 </sst>
 </file>
@@ -8052,8 +8055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B829" workbookViewId="0">
-      <selection activeCell="F853" sqref="F853"/>
+    <sheetView tabSelected="1" topLeftCell="A839" workbookViewId="0">
+      <selection activeCell="F869" sqref="F869"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8061,7 +8064,7 @@
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="54.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
@@ -20060,6 +20063,9 @@
       <c r="D853" t="s">
         <v>494</v>
       </c>
+      <c r="F853" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="854" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
@@ -20074,6 +20080,9 @@
       <c r="D854" t="s">
         <v>494</v>
       </c>
+      <c r="F854" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="855" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
@@ -20088,6 +20097,9 @@
       <c r="D855" t="s">
         <v>1363</v>
       </c>
+      <c r="F855" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
@@ -20102,6 +20114,9 @@
       <c r="D856" t="s">
         <v>400</v>
       </c>
+      <c r="F856" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="857" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
@@ -20116,6 +20131,9 @@
       <c r="D857" t="s">
         <v>1364</v>
       </c>
+      <c r="F857" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="858" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
@@ -20130,6 +20148,12 @@
       <c r="D858" t="s">
         <v>1365</v>
       </c>
+      <c r="F858" t="s">
+        <v>2400</v>
+      </c>
+      <c r="I858" t="s">
+        <v>2404</v>
+      </c>
     </row>
     <row r="859" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
@@ -20144,6 +20168,9 @@
       <c r="D859" t="s">
         <v>1132</v>
       </c>
+      <c r="F859" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="860" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
@@ -20158,6 +20185,9 @@
       <c r="D860" t="s">
         <v>1132</v>
       </c>
+      <c r="F860" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="861" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
@@ -20172,6 +20202,9 @@
       <c r="D861" t="s">
         <v>400</v>
       </c>
+      <c r="F861" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
@@ -20186,6 +20219,9 @@
       <c r="D862" t="s">
         <v>1577</v>
       </c>
+      <c r="F862" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="863" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
@@ -20200,6 +20236,9 @@
       <c r="D863" t="s">
         <v>794</v>
       </c>
+      <c r="F863" t="s">
+        <v>2400</v>
+      </c>
     </row>
     <row r="864" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
@@ -20214,8 +20253,11 @@
       <c r="D864" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="865" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F864" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="865" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
         <v>1349</v>
       </c>
@@ -20228,8 +20270,11 @@
       <c r="D865" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="866" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F865" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="866" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
         <v>1350</v>
       </c>
@@ -20242,8 +20287,11 @@
       <c r="D866" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="867" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F866" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="867" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
         <v>1351</v>
       </c>
@@ -20256,8 +20304,11 @@
       <c r="D867" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="868" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F867" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="868" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
         <v>1352</v>
       </c>
@@ -20270,8 +20321,11 @@
       <c r="D868" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="869" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F868" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="869" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
         <v>1353</v>
       </c>
@@ -20284,8 +20338,11 @@
       <c r="D869" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="870" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F869" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="870" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
         <v>1354</v>
       </c>
@@ -20299,7 +20356,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="871" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
         <v>1367</v>
       </c>
@@ -20313,7 +20370,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="872" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
         <v>1368</v>
       </c>
@@ -20327,7 +20384,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="873" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
         <v>1369</v>
       </c>
@@ -20341,7 +20398,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="874" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
         <v>1370</v>
       </c>
@@ -20355,7 +20412,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="875" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
         <v>1371</v>
       </c>
@@ -20369,7 +20426,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="876" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
         <v>1372</v>
       </c>
@@ -20383,7 +20440,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="877" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
         <v>1373</v>
       </c>
@@ -20397,7 +20454,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="878" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
         <v>1374</v>
       </c>
@@ -20411,7 +20468,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="879" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
         <v>1375</v>
       </c>
@@ -20425,7 +20482,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="880" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
         <v>1376</v>
       </c>

</xml_diff>